<commit_message>
Correction dico et matrice
</commit_message>
<xml_diff>
--- a/merise/cas_horse/cas_horse.xlsx
+++ b/merise/cas_horse/cas_horse.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="matrice" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="26">
   <si>
     <t>Horse</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>company_name</t>
+  </si>
+  <si>
+    <t>company_siren_number</t>
   </si>
 </sst>
 </file>
@@ -414,6 +417,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -425,9 +431,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -732,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -759,10 +762,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +805,7 @@
       <c r="O1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="P1" s="29" t="s">
         <v>19</v>
       </c>
       <c r="Q1" s="28" t="s">
@@ -810,8 +813,8 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -1257,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -1282,10 +1285,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1293,7 +1296,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -1307,8 +1310,8 @@
       <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -1316,7 +1319,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>

</xml_diff>

<commit_message>
exo cas Horse P2 suite
</commit_message>
<xml_diff>
--- a/merise/cas_horse/cas_horse.xlsx
+++ b/merise/cas_horse/cas_horse.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="matrice" sheetId="1" r:id="rId1"/>
     <sheet name="matrice simplifiée" sheetId="4" r:id="rId2"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId3"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId4"/>
+    <sheet name="matrice p2" sheetId="2" r:id="rId3"/>
+    <sheet name="matrice p2 simplifié" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="43">
   <si>
     <t>Horse</t>
   </si>
@@ -95,13 +95,64 @@
   </si>
   <si>
     <t>company_siren_number</t>
+  </si>
+  <si>
+    <t>races_meeting</t>
+  </si>
+  <si>
+    <t>meeting_id</t>
+  </si>
+  <si>
+    <t>races</t>
+  </si>
+  <si>
+    <t>race_id</t>
+  </si>
+  <si>
+    <t>race_number</t>
+  </si>
+  <si>
+    <t>race_name_trial</t>
+  </si>
+  <si>
+    <t>race_distance</t>
+  </si>
+  <si>
+    <t>race_type</t>
+  </si>
+  <si>
+    <t>race_start_time</t>
+  </si>
+  <si>
+    <t>race_price_win</t>
+  </si>
+  <si>
+    <t>horse_parents</t>
+  </si>
+  <si>
+    <t>parent_id</t>
+  </si>
+  <si>
+    <t>parent_gender</t>
+  </si>
+  <si>
+    <t>parent_name</t>
+  </si>
+  <si>
+    <t>meeting_start_time</t>
+  </si>
+  <si>
+    <t>racetracks</t>
+  </si>
+  <si>
+    <t>racetrack_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +222,81 @@
     <font>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF8064A2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF8064A2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF948A54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF948A54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF953735"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF953735"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF4BACC6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4BACC6"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -331,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -419,6 +545,64 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -736,7 +920,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -762,10 +946,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="53"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -813,8 +997,8 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="33"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="55"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -1260,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -1285,10 +1469,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="53"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1310,8 +1494,8 @@
       <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="33"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="55"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -1668,24 +1852,1897 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AE36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N137" sqref="N137"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB1" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC1" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD1" s="47" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="54"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="W2" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z2" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA2" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB2" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC2" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD2" s="48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="31"/>
+    </row>
+    <row r="4" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="31"/>
+    </row>
+    <row r="5" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="31"/>
+    </row>
+    <row r="6" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="31"/>
+      <c r="AE6" s="30"/>
+    </row>
+    <row r="7" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="31"/>
+      <c r="AE7" s="45"/>
+    </row>
+    <row r="8" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="31"/>
+      <c r="AE8" s="30"/>
+    </row>
+    <row r="9" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="31"/>
+      <c r="AE9" s="30"/>
+    </row>
+    <row r="10" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="31"/>
+      <c r="AE10" s="30"/>
+    </row>
+    <row r="11" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="31"/>
+      <c r="AE11" s="30"/>
+    </row>
+    <row r="12" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6">
+        <v>1</v>
+      </c>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="31"/>
+    </row>
+    <row r="13" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6">
+        <v>1</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="31"/>
+    </row>
+    <row r="14" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6">
+        <v>1</v>
+      </c>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="31"/>
+    </row>
+    <row r="15" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="31"/>
+    </row>
+    <row r="16" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="31"/>
+    </row>
+    <row r="17" spans="1:30" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="31"/>
+    </row>
+    <row r="18" spans="1:30" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="6"/>
+      <c r="AD18" s="31"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
+      <c r="AA19" s="6"/>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="6"/>
+      <c r="AD19" s="31"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6">
+        <v>1</v>
+      </c>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="31"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A21" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="6"/>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="31"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6">
+        <v>1</v>
+      </c>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
+      <c r="AA22" s="6"/>
+      <c r="AB22" s="6"/>
+      <c r="AC22" s="6"/>
+      <c r="AD22" s="31"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6">
+        <v>1</v>
+      </c>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="6"/>
+      <c r="AC23" s="6"/>
+      <c r="AD23" s="31"/>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6">
+        <v>1</v>
+      </c>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="6"/>
+      <c r="AA24" s="6"/>
+      <c r="AB24" s="6"/>
+      <c r="AC24" s="6"/>
+      <c r="AD24" s="31"/>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6">
+        <v>1</v>
+      </c>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
+      <c r="AA25" s="6"/>
+      <c r="AB25" s="6"/>
+      <c r="AC25" s="6"/>
+      <c r="AD25" s="31"/>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6">
+        <v>1</v>
+      </c>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
+      <c r="X26" s="6"/>
+      <c r="Y26" s="6"/>
+      <c r="Z26" s="6"/>
+      <c r="AA26" s="6"/>
+      <c r="AB26" s="6"/>
+      <c r="AC26" s="6"/>
+      <c r="AD26" s="31"/>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A27" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6">
+        <v>1</v>
+      </c>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="6"/>
+      <c r="AC27" s="6"/>
+      <c r="AD27" s="31"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A28" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="6"/>
+      <c r="Y28" s="6"/>
+      <c r="Z28" s="6"/>
+      <c r="AA28" s="6"/>
+      <c r="AB28" s="6"/>
+      <c r="AC28" s="6"/>
+      <c r="AD28" s="31"/>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A29" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
+      <c r="V29" s="6"/>
+      <c r="W29" s="6"/>
+      <c r="X29" s="6"/>
+      <c r="Y29" s="6"/>
+      <c r="Z29" s="6"/>
+      <c r="AA29" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB29" s="6"/>
+      <c r="AC29" s="6"/>
+      <c r="AD29" s="31"/>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A30" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="6"/>
+      <c r="Y30" s="6"/>
+      <c r="Z30" s="6"/>
+      <c r="AA30" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB30" s="6"/>
+      <c r="AC30" s="6"/>
+      <c r="AD30" s="31"/>
+    </row>
+    <row r="31" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="32"/>
+      <c r="Q31" s="32"/>
+      <c r="R31" s="32"/>
+      <c r="S31" s="32"/>
+      <c r="T31" s="32"/>
+      <c r="U31" s="32"/>
+      <c r="V31" s="32"/>
+      <c r="W31" s="32"/>
+      <c r="X31" s="32"/>
+      <c r="Y31" s="32"/>
+      <c r="Z31" s="32"/>
+      <c r="AA31" s="32"/>
+      <c r="AB31" s="32"/>
+      <c r="AC31" s="32"/>
+      <c r="AD31" s="33"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="44"/>
+      <c r="C35" s="45"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="47" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="54"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="31"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="31"/>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="31"/>
+    </row>
+    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="30"/>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="45"/>
+    </row>
+    <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="30"/>
+    </row>
+    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="30"/>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="30"/>
+    </row>
+    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="30"/>
+    </row>
+    <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="31"/>
+    </row>
+    <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="31"/>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6">
+        <v>1</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="31"/>
+    </row>
+    <row r="15" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="31"/>
+    </row>
+    <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="31"/>
+    </row>
+    <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="31"/>
+    </row>
+    <row r="18" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="31"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="31"/>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6">
+        <v>1</v>
+      </c>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="31"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="31"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6">
+        <v>1</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="31"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6">
+        <v>1</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="31"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6">
+        <v>1</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="31"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6">
+        <v>1</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="31"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6">
+        <v>1</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="31"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6">
+        <v>1</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="31"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="31"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6">
+        <v>1</v>
+      </c>
+      <c r="I29" s="31"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6">
+        <v>1</v>
+      </c>
+      <c r="I30" s="31"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="33"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="44"/>
+      <c r="C35" s="45"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Horse partie 2
</commit_message>
<xml_diff>
--- a/merise/cas_horse/cas_horse.xlsx
+++ b/merise/cas_horse/cas_horse.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="matrice" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="51">
   <si>
     <t>Horse</t>
   </si>
@@ -146,13 +146,37 @@
   </si>
   <si>
     <t>racetrack_name</t>
+  </si>
+  <si>
+    <t>horse_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>horse_handicap_weight</t>
+  </si>
+  <si>
+    <t>horse_handicap_distance</t>
+  </si>
+  <si>
+    <t>horse_starting_block</t>
+  </si>
+  <si>
+    <t>horse_name</t>
+  </si>
+  <si>
+    <t>horse_type</t>
+  </si>
+  <si>
+    <t>person_stable_color</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,6 +325,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4F81BD"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -310,7 +341,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -453,11 +484,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -615,6 +683,67 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1852,133 +1981,110 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE36"/>
+  <dimension ref="A1:AL43"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N137" sqref="N137"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14" customWidth="1"/>
-    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="31" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.28515625" customWidth="1"/>
+    <col min="33" max="33" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="53"/>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="29" t="s">
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" s="34" t="s">
+      <c r="S1" s="57"/>
+      <c r="T1" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" s="35" t="s">
+      <c r="U1" s="58"/>
+      <c r="V1" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="V1" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="W1" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="X1" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y1" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z1" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA1" s="41" t="s">
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="59"/>
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="AB1" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC1" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD1" s="47" t="s">
+      <c r="AD1" s="60"/>
+      <c r="AE1" s="60"/>
+      <c r="AF1" s="72" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="AG1" s="74"/>
+      <c r="AH1" s="75"/>
+      <c r="AI1" s="75"/>
+      <c r="AJ1" s="75"/>
+      <c r="AK1" s="75"/>
+      <c r="AL1" s="76"/>
+    </row>
+    <row r="2" spans="1:38" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="54"/>
       <c r="B2" s="55"/>
       <c r="C2" s="14" t="s">
@@ -1997,77 +2103,101 @@
         <v>6</v>
       </c>
       <c r="H2" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="K2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="L2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="M2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="N2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="O2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="P2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="26" t="s">
+      <c r="Q2" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="R2" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="26" t="s">
+      <c r="S2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="36" t="s">
+      <c r="T2" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="S2" s="46" t="s">
+      <c r="U2" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="37" t="s">
+      <c r="V2" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="U2" s="37" t="s">
+      <c r="W2" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="V2" s="37" t="s">
+      <c r="X2" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="W2" s="37" t="s">
+      <c r="Y2" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="X2" s="37" t="s">
+      <c r="Z2" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Y2" s="37" t="s">
+      <c r="AA2" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="Z2" s="37" t="s">
+      <c r="AB2" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="AA2" s="42" t="s">
+      <c r="AC2" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="AB2" s="42" t="s">
+      <c r="AD2" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="AC2" s="42" t="s">
+      <c r="AE2" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="AD2" s="48" t="s">
+      <c r="AF2" s="69" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="AG2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI2" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ2" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK2" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL2" s="73" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="61" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -2100,12 +2230,18 @@
       <c r="AA3" s="6"/>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
-      <c r="AD3" s="31"/>
-    </row>
-    <row r="4" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="67"/>
+      <c r="AG3" s="67"/>
+      <c r="AH3" s="67"/>
+      <c r="AI3" s="67"/>
+      <c r="AJ3" s="67"/>
+      <c r="AK3" s="67"/>
+      <c r="AL3" s="31"/>
+    </row>
+    <row r="4" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="61"/>
       <c r="B4" s="14" t="s">
         <v>3</v>
       </c>
@@ -2138,12 +2274,18 @@
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
-      <c r="AD4" s="31"/>
-    </row>
-    <row r="5" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="67"/>
+      <c r="AG4" s="67"/>
+      <c r="AH4" s="67"/>
+      <c r="AI4" s="67"/>
+      <c r="AJ4" s="67"/>
+      <c r="AK4" s="67"/>
+      <c r="AL4" s="31"/>
+    </row>
+    <row r="5" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="61"/>
       <c r="B5" s="14" t="s">
         <v>4</v>
       </c>
@@ -2176,12 +2318,18 @@
       <c r="AA5" s="6"/>
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
-      <c r="AD5" s="31"/>
-    </row>
-    <row r="6" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="67"/>
+      <c r="AG5" s="67"/>
+      <c r="AH5" s="67"/>
+      <c r="AI5" s="67"/>
+      <c r="AJ5" s="67"/>
+      <c r="AK5" s="67"/>
+      <c r="AL5" s="31"/>
+    </row>
+    <row r="6" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="61"/>
       <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
@@ -2214,13 +2362,18 @@
       <c r="AA6" s="6"/>
       <c r="AB6" s="6"/>
       <c r="AC6" s="6"/>
-      <c r="AD6" s="31"/>
-      <c r="AE6" s="30"/>
-    </row>
-    <row r="7" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="67"/>
+      <c r="AG6" s="67"/>
+      <c r="AH6" s="67"/>
+      <c r="AI6" s="67"/>
+      <c r="AJ6" s="67"/>
+      <c r="AK6" s="67"/>
+      <c r="AL6" s="31"/>
+    </row>
+    <row r="7" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="61"/>
       <c r="B7" s="14" t="s">
         <v>6</v>
       </c>
@@ -2253,15 +2406,20 @@
       <c r="AA7" s="6"/>
       <c r="AB7" s="6"/>
       <c r="AC7" s="6"/>
-      <c r="AD7" s="31"/>
-      <c r="AE7" s="45"/>
-    </row>
-    <row r="8" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="67"/>
+      <c r="AG7" s="46"/>
+      <c r="AH7" s="67"/>
+      <c r="AI7" s="67"/>
+      <c r="AJ7" s="67"/>
+      <c r="AK7" s="67"/>
+      <c r="AL7" s="31"/>
+    </row>
+    <row r="8" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="61"/>
       <c r="B8" s="14" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C8" s="6">
         <v>1</v>
@@ -2292,15 +2450,20 @@
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
       <c r="AC8" s="6"/>
-      <c r="AD8" s="31"/>
-      <c r="AE8" s="30"/>
-    </row>
-    <row r="9" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>8</v>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="67"/>
+      <c r="AG8" s="46"/>
+      <c r="AH8" s="67"/>
+      <c r="AI8" s="67"/>
+      <c r="AJ8" s="67"/>
+      <c r="AK8" s="67"/>
+      <c r="AL8" s="31"/>
+    </row>
+    <row r="9" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="61"/>
+      <c r="B9" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="C9" s="6">
         <v>1</v>
@@ -2331,25 +2494,30 @@
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
       <c r="AC9" s="6"/>
-      <c r="AD9" s="31"/>
-      <c r="AE9" s="30"/>
-    </row>
-    <row r="10" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="6"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="67"/>
+      <c r="AG9" s="46"/>
+      <c r="AH9" s="67"/>
+      <c r="AI9" s="67"/>
+      <c r="AJ9" s="67"/>
+      <c r="AK9" s="67"/>
+      <c r="AL9" s="31"/>
+    </row>
+    <row r="10" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="61"/>
+      <c r="B10" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="6">
-        <v>1</v>
-      </c>
+      <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -2370,25 +2538,32 @@
       <c r="AA10" s="6"/>
       <c r="AB10" s="6"/>
       <c r="AC10" s="6"/>
-      <c r="AD10" s="31"/>
-      <c r="AE10" s="30"/>
-    </row>
-    <row r="11" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="AD10" s="6"/>
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="67"/>
+      <c r="AG10" s="67"/>
+      <c r="AH10" s="67"/>
+      <c r="AI10" s="67"/>
+      <c r="AJ10" s="67"/>
+      <c r="AK10" s="67"/>
+      <c r="AL10" s="31"/>
+    </row>
+    <row r="11" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="62" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="6"/>
+        <v>8</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="6">
-        <v>1</v>
-      </c>
+      <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -2409,15 +2584,20 @@
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
       <c r="AC11" s="6"/>
-      <c r="AD11" s="31"/>
-      <c r="AE11" s="30"/>
-    </row>
-    <row r="12" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="AD11" s="6"/>
+      <c r="AE11" s="6"/>
+      <c r="AF11" s="67"/>
+      <c r="AG11" s="67"/>
+      <c r="AH11" s="67"/>
+      <c r="AI11" s="67"/>
+      <c r="AJ11" s="67"/>
+      <c r="AK11" s="67"/>
+      <c r="AL11" s="31"/>
+    </row>
+    <row r="12" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="62"/>
       <c r="B12" s="15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -2425,11 +2605,11 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="6">
-        <v>1</v>
-      </c>
+      <c r="I12" s="6"/>
       <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="K12" s="6">
+        <v>1</v>
+      </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
@@ -2448,14 +2628,20 @@
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
       <c r="AC12" s="6"/>
-      <c r="AD12" s="31"/>
-    </row>
-    <row r="13" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="AD12" s="6"/>
+      <c r="AE12" s="6"/>
+      <c r="AF12" s="67"/>
+      <c r="AG12" s="67"/>
+      <c r="AH12" s="67"/>
+      <c r="AI12" s="67"/>
+      <c r="AJ12" s="67"/>
+      <c r="AK12" s="67"/>
+      <c r="AL12" s="31"/>
+    </row>
+    <row r="13" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="62"/>
       <c r="B13" s="15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -2463,11 +2649,11 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="6">
-        <v>1</v>
-      </c>
+      <c r="I13" s="6"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+      <c r="K13" s="6">
+        <v>1</v>
+      </c>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
@@ -2486,14 +2672,20 @@
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
       <c r="AC13" s="6"/>
-      <c r="AD13" s="31"/>
-    </row>
-    <row r="14" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="AD13" s="6"/>
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="67"/>
+      <c r="AG13" s="67"/>
+      <c r="AH13" s="67"/>
+      <c r="AI13" s="67"/>
+      <c r="AJ13" s="67"/>
+      <c r="AK13" s="67"/>
+      <c r="AL13" s="31"/>
+    </row>
+    <row r="14" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="62"/>
       <c r="B14" s="15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2501,11 +2693,11 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="6">
-        <v>1</v>
-      </c>
+      <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="K14" s="6">
+        <v>1</v>
+      </c>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
@@ -2524,28 +2716,36 @@
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
       <c r="AC14" s="6"/>
-      <c r="AD14" s="31"/>
-    </row>
-    <row r="15" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
+      <c r="AD14" s="6"/>
+      <c r="AE14" s="6"/>
+      <c r="AF14" s="67"/>
+      <c r="AG14" s="67"/>
+      <c r="AH14" s="67"/>
+      <c r="AI14" s="67"/>
+      <c r="AJ14" s="67"/>
+      <c r="AK14" s="67"/>
+      <c r="AL14" s="31"/>
+    </row>
+    <row r="15" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="62"/>
+      <c r="B15" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6">
+        <v>1</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
@@ -2560,14 +2760,20 @@
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
       <c r="AC15" s="6"/>
-      <c r="AD15" s="31"/>
-    </row>
-    <row r="16" spans="1:31" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>24</v>
+      <c r="AD15" s="6"/>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="67"/>
+      <c r="AG15" s="67"/>
+      <c r="AH15" s="67"/>
+      <c r="AI15" s="67"/>
+      <c r="AJ15" s="67"/>
+      <c r="AK15" s="67"/>
+      <c r="AL15" s="31"/>
+    </row>
+    <row r="16" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="62"/>
+      <c r="B16" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -2577,14 +2783,14 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
+      <c r="K16" s="6">
+        <v>1</v>
+      </c>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
-      <c r="P16" s="6">
-        <v>1</v>
-      </c>
+      <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
@@ -2598,12 +2804,20 @@
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
       <c r="AC16" s="6"/>
-      <c r="AD16" s="31"/>
-    </row>
-    <row r="17" spans="1:30" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="23" t="s">
-        <v>17</v>
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="6"/>
+      <c r="AF16" s="67"/>
+      <c r="AG16" s="67"/>
+      <c r="AH16" s="67"/>
+      <c r="AI16" s="67"/>
+      <c r="AJ16" s="67"/>
+      <c r="AK16" s="67"/>
+      <c r="AL16" s="31"/>
+    </row>
+    <row r="17" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="71" t="s">
+        <v>50</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2632,28 +2846,38 @@
       <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
       <c r="AC17" s="6"/>
-      <c r="AD17" s="31"/>
-    </row>
-    <row r="18" spans="1:30" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="6"/>
+      <c r="AF17" s="67"/>
+      <c r="AG17" s="67"/>
+      <c r="AH17" s="67"/>
+      <c r="AI17" s="67"/>
+      <c r="AJ17" s="67"/>
+      <c r="AK17" s="67"/>
+      <c r="AL17" s="31"/>
+    </row>
+    <row r="18" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
@@ -2666,14 +2890,20 @@
       <c r="AA18" s="6"/>
       <c r="AB18" s="6"/>
       <c r="AC18" s="6"/>
-      <c r="AD18" s="31"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A19" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="36" t="s">
-        <v>27</v>
+      <c r="AD18" s="6"/>
+      <c r="AE18" s="6"/>
+      <c r="AF18" s="67"/>
+      <c r="AG18" s="67"/>
+      <c r="AH18" s="67"/>
+      <c r="AI18" s="67"/>
+      <c r="AJ18" s="67"/>
+      <c r="AK18" s="67"/>
+      <c r="AL18" s="31"/>
+    </row>
+    <row r="19" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="63"/>
+      <c r="B19" s="26" t="s">
+        <v>24</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -2690,7 +2920,9 @@
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
+      <c r="R19" s="6">
+        <v>1</v>
+      </c>
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
       <c r="U19" s="6"/>
@@ -2702,16 +2934,26 @@
       <c r="AA19" s="6"/>
       <c r="AB19" s="6"/>
       <c r="AC19" s="6"/>
-      <c r="AD19" s="31"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A20" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="6"/>
+      <c r="AD19" s="6"/>
+      <c r="AE19" s="6"/>
+      <c r="AF19" s="67"/>
+      <c r="AG19" s="67"/>
+      <c r="AH19" s="67"/>
+      <c r="AI19" s="67"/>
+      <c r="AJ19" s="67"/>
+      <c r="AK19" s="67"/>
+      <c r="AL19" s="31"/>
+    </row>
+    <row r="20" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -2719,16 +2961,16 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
+      <c r="K20" s="6">
+        <v>1</v>
+      </c>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
-      <c r="R20" s="6">
-        <v>1</v>
-      </c>
+      <c r="R20" s="6"/>
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
       <c r="U20" s="6"/>
@@ -2740,16 +2982,24 @@
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
       <c r="AC20" s="6"/>
-      <c r="AD20" s="31"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="6"/>
+      <c r="AD20" s="6"/>
+      <c r="AE20" s="6"/>
+      <c r="AF20" s="67"/>
+      <c r="AG20" s="67"/>
+      <c r="AH20" s="67"/>
+      <c r="AI20" s="67"/>
+      <c r="AJ20" s="67"/>
+      <c r="AK20" s="67"/>
+      <c r="AL20" s="31"/>
+    </row>
+    <row r="21" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="68"/>
+      <c r="B21" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="6">
+        <v>1</v>
+      </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -2757,7 +3007,9 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
+      <c r="K21" s="6">
+        <v>1</v>
+      </c>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
@@ -2776,14 +3028,20 @@
       <c r="AA21" s="6"/>
       <c r="AB21" s="6"/>
       <c r="AC21" s="6"/>
-      <c r="AD21" s="31"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="40" t="s">
-        <v>30</v>
+      <c r="AD21" s="6"/>
+      <c r="AE21" s="6"/>
+      <c r="AF21" s="67"/>
+      <c r="AG21" s="67"/>
+      <c r="AH21" s="67"/>
+      <c r="AI21" s="67"/>
+      <c r="AJ21" s="67"/>
+      <c r="AK21" s="67"/>
+      <c r="AL21" s="31"/>
+    </row>
+    <row r="22" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="68"/>
+      <c r="B22" s="23" t="s">
+        <v>45</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -2803,9 +3061,7 @@
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
-      <c r="U22" s="6">
-        <v>1</v>
-      </c>
+      <c r="U22" s="6"/>
       <c r="V22" s="6"/>
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
@@ -2814,14 +3070,20 @@
       <c r="AA22" s="6"/>
       <c r="AB22" s="6"/>
       <c r="AC22" s="6"/>
-      <c r="AD22" s="31"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="40" t="s">
-        <v>31</v>
+      <c r="AD22" s="6"/>
+      <c r="AE22" s="6"/>
+      <c r="AF22" s="67"/>
+      <c r="AG22" s="67"/>
+      <c r="AH22" s="67"/>
+      <c r="AI22" s="67"/>
+      <c r="AJ22" s="67"/>
+      <c r="AK22" s="67"/>
+      <c r="AL22" s="31"/>
+    </row>
+    <row r="23" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="68"/>
+      <c r="B23" s="23" t="s">
+        <v>46</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -2841,9 +3103,7 @@
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
-      <c r="U23" s="6">
-        <v>1</v>
-      </c>
+      <c r="U23" s="6"/>
       <c r="V23" s="6"/>
       <c r="W23" s="6"/>
       <c r="X23" s="6"/>
@@ -2852,14 +3112,20 @@
       <c r="AA23" s="6"/>
       <c r="AB23" s="6"/>
       <c r="AC23" s="6"/>
-      <c r="AD23" s="31"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A24" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="40" t="s">
-        <v>32</v>
+      <c r="AD23" s="6"/>
+      <c r="AE23" s="6"/>
+      <c r="AF23" s="67"/>
+      <c r="AG23" s="67"/>
+      <c r="AH23" s="67"/>
+      <c r="AI23" s="67"/>
+      <c r="AJ23" s="67"/>
+      <c r="AK23" s="67"/>
+      <c r="AL23" s="31"/>
+    </row>
+    <row r="24" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="68"/>
+      <c r="B24" s="23" t="s">
+        <v>43</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -2879,9 +3145,7 @@
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
       <c r="T24" s="6"/>
-      <c r="U24" s="6">
-        <v>1</v>
-      </c>
+      <c r="U24" s="6"/>
       <c r="V24" s="6"/>
       <c r="W24" s="6"/>
       <c r="X24" s="6"/>
@@ -2890,14 +3154,20 @@
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
       <c r="AC24" s="6"/>
-      <c r="AD24" s="31"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="40" t="s">
-        <v>33</v>
+      <c r="AD24" s="6"/>
+      <c r="AE24" s="6"/>
+      <c r="AF24" s="67"/>
+      <c r="AG24" s="67"/>
+      <c r="AH24" s="67"/>
+      <c r="AI24" s="67"/>
+      <c r="AJ24" s="67"/>
+      <c r="AK24" s="67"/>
+      <c r="AL24" s="31"/>
+    </row>
+    <row r="25" spans="1:38" s="30" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="68"/>
+      <c r="B25" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -2917,9 +3187,7 @@
       <c r="R25" s="6"/>
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
-      <c r="U25" s="6">
-        <v>1</v>
-      </c>
+      <c r="U25" s="6"/>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
@@ -2928,14 +3196,22 @@
       <c r="AA25" s="6"/>
       <c r="AB25" s="6"/>
       <c r="AC25" s="6"/>
-      <c r="AD25" s="31"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A26" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="40" t="s">
-        <v>34</v>
+      <c r="AD25" s="6"/>
+      <c r="AE25" s="6"/>
+      <c r="AF25" s="67"/>
+      <c r="AG25" s="67"/>
+      <c r="AH25" s="67"/>
+      <c r="AI25" s="67"/>
+      <c r="AJ25" s="67"/>
+      <c r="AK25" s="67"/>
+      <c r="AL25" s="31"/>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A26" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>27</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -2955,9 +3231,7 @@
       <c r="R26" s="6"/>
       <c r="S26" s="6"/>
       <c r="T26" s="6"/>
-      <c r="U26" s="6">
-        <v>1</v>
-      </c>
+      <c r="U26" s="6"/>
       <c r="V26" s="6"/>
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
@@ -2966,14 +3240,20 @@
       <c r="AA26" s="6"/>
       <c r="AB26" s="6"/>
       <c r="AC26" s="6"/>
-      <c r="AD26" s="31"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A27" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="40" t="s">
-        <v>35</v>
+      <c r="AD26" s="6"/>
+      <c r="AE26" s="6"/>
+      <c r="AF26" s="67"/>
+      <c r="AG26" s="67"/>
+      <c r="AH26" s="67"/>
+      <c r="AI26" s="67"/>
+      <c r="AJ26" s="67"/>
+      <c r="AK26" s="67"/>
+      <c r="AL26" s="31"/>
+    </row>
+    <row r="27" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="64"/>
+      <c r="B27" s="46" t="s">
+        <v>40</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -2992,10 +3272,10 @@
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
       <c r="S27" s="6"/>
-      <c r="T27" s="6"/>
-      <c r="U27" s="6">
-        <v>1</v>
-      </c>
+      <c r="T27" s="6">
+        <v>1</v>
+      </c>
+      <c r="U27" s="6"/>
       <c r="V27" s="6"/>
       <c r="W27" s="6"/>
       <c r="X27" s="6"/>
@@ -3004,14 +3284,22 @@
       <c r="AA27" s="6"/>
       <c r="AB27" s="6"/>
       <c r="AC27" s="6"/>
-      <c r="AD27" s="31"/>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A28" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="42" t="s">
-        <v>37</v>
+      <c r="AD27" s="6"/>
+      <c r="AE27" s="6"/>
+      <c r="AF27" s="67"/>
+      <c r="AG27" s="67"/>
+      <c r="AH27" s="67"/>
+      <c r="AI27" s="67"/>
+      <c r="AJ27" s="67"/>
+      <c r="AK27" s="67"/>
+      <c r="AL27" s="31"/>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A28" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>29</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -3040,14 +3328,20 @@
       <c r="AA28" s="6"/>
       <c r="AB28" s="6"/>
       <c r="AC28" s="6"/>
-      <c r="AD28" s="31"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A29" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="42" t="s">
-        <v>38</v>
+      <c r="AD28" s="6"/>
+      <c r="AE28" s="6"/>
+      <c r="AF28" s="67"/>
+      <c r="AG28" s="67"/>
+      <c r="AH28" s="67"/>
+      <c r="AI28" s="67"/>
+      <c r="AJ28" s="67"/>
+      <c r="AK28" s="67"/>
+      <c r="AL28" s="31"/>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A29" s="65"/>
+      <c r="B29" s="40" t="s">
+        <v>30</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -3069,23 +3363,29 @@
       <c r="T29" s="6"/>
       <c r="U29" s="6"/>
       <c r="V29" s="6"/>
-      <c r="W29" s="6"/>
+      <c r="W29" s="6">
+        <v>1</v>
+      </c>
       <c r="X29" s="6"/>
       <c r="Y29" s="6"/>
       <c r="Z29" s="6"/>
-      <c r="AA29" s="6">
-        <v>1</v>
-      </c>
+      <c r="AA29" s="6"/>
       <c r="AB29" s="6"/>
       <c r="AC29" s="6"/>
-      <c r="AD29" s="31"/>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A30" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="42" t="s">
-        <v>39</v>
+      <c r="AD29" s="6"/>
+      <c r="AE29" s="6"/>
+      <c r="AF29" s="67"/>
+      <c r="AG29" s="67"/>
+      <c r="AH29" s="67"/>
+      <c r="AI29" s="67"/>
+      <c r="AJ29" s="67"/>
+      <c r="AK29" s="67"/>
+      <c r="AL29" s="31"/>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A30" s="65"/>
+      <c r="B30" s="40" t="s">
+        <v>31</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -3107,68 +3407,406 @@
       <c r="T30" s="6"/>
       <c r="U30" s="6"/>
       <c r="V30" s="6"/>
-      <c r="W30" s="6"/>
+      <c r="W30" s="6">
+        <v>1</v>
+      </c>
       <c r="X30" s="6"/>
       <c r="Y30" s="6"/>
       <c r="Z30" s="6"/>
-      <c r="AA30" s="6">
-        <v>1</v>
-      </c>
+      <c r="AA30" s="6"/>
       <c r="AB30" s="6"/>
       <c r="AC30" s="6"/>
-      <c r="AD30" s="31"/>
-    </row>
-    <row r="31" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="50" t="s">
+      <c r="AD30" s="6"/>
+      <c r="AE30" s="6"/>
+      <c r="AF30" s="67"/>
+      <c r="AG30" s="67"/>
+      <c r="AH30" s="67"/>
+      <c r="AI30" s="67"/>
+      <c r="AJ30" s="67"/>
+      <c r="AK30" s="67"/>
+      <c r="AL30" s="31"/>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A31" s="65"/>
+      <c r="B31" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="6"/>
+      <c r="U31" s="6"/>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6">
+        <v>1</v>
+      </c>
+      <c r="X31" s="6"/>
+      <c r="Y31" s="6"/>
+      <c r="Z31" s="6"/>
+      <c r="AA31" s="6"/>
+      <c r="AB31" s="6"/>
+      <c r="AC31" s="6"/>
+      <c r="AD31" s="6"/>
+      <c r="AE31" s="6"/>
+      <c r="AF31" s="67"/>
+      <c r="AG31" s="67"/>
+      <c r="AH31" s="67"/>
+      <c r="AI31" s="67"/>
+      <c r="AJ31" s="67"/>
+      <c r="AK31" s="67"/>
+      <c r="AL31" s="31"/>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A32" s="65"/>
+      <c r="B32" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="6"/>
+      <c r="U32" s="6"/>
+      <c r="V32" s="6"/>
+      <c r="W32" s="6">
+        <v>1</v>
+      </c>
+      <c r="X32" s="6"/>
+      <c r="Y32" s="6"/>
+      <c r="Z32" s="6"/>
+      <c r="AA32" s="6"/>
+      <c r="AB32" s="6"/>
+      <c r="AC32" s="6"/>
+      <c r="AD32" s="6"/>
+      <c r="AE32" s="6"/>
+      <c r="AF32" s="67"/>
+      <c r="AG32" s="67"/>
+      <c r="AH32" s="67"/>
+      <c r="AI32" s="67"/>
+      <c r="AJ32" s="67"/>
+      <c r="AK32" s="67"/>
+      <c r="AL32" s="31"/>
+    </row>
+    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A33" s="65"/>
+      <c r="B33" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6"/>
+      <c r="T33" s="6"/>
+      <c r="U33" s="6"/>
+      <c r="V33" s="6"/>
+      <c r="W33" s="6">
+        <v>1</v>
+      </c>
+      <c r="X33" s="6"/>
+      <c r="Y33" s="6"/>
+      <c r="Z33" s="6"/>
+      <c r="AA33" s="6"/>
+      <c r="AB33" s="6"/>
+      <c r="AC33" s="6"/>
+      <c r="AD33" s="6"/>
+      <c r="AE33" s="6"/>
+      <c r="AF33" s="67"/>
+      <c r="AG33" s="67"/>
+      <c r="AH33" s="67"/>
+      <c r="AI33" s="67"/>
+      <c r="AJ33" s="67"/>
+      <c r="AK33" s="67"/>
+      <c r="AL33" s="31"/>
+    </row>
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A34" s="65"/>
+      <c r="B34" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="6"/>
+      <c r="U34" s="6"/>
+      <c r="V34" s="6"/>
+      <c r="W34" s="6">
+        <v>1</v>
+      </c>
+      <c r="X34" s="6"/>
+      <c r="Y34" s="6"/>
+      <c r="Z34" s="6"/>
+      <c r="AA34" s="6"/>
+      <c r="AB34" s="6"/>
+      <c r="AC34" s="6"/>
+      <c r="AD34" s="6"/>
+      <c r="AE34" s="6"/>
+      <c r="AF34" s="67"/>
+      <c r="AG34" s="67"/>
+      <c r="AH34" s="67"/>
+      <c r="AI34" s="67"/>
+      <c r="AJ34" s="67"/>
+      <c r="AK34" s="67"/>
+      <c r="AL34" s="31"/>
+    </row>
+    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A35" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6"/>
+      <c r="T35" s="6"/>
+      <c r="U35" s="6"/>
+      <c r="V35" s="6"/>
+      <c r="W35" s="6"/>
+      <c r="X35" s="6"/>
+      <c r="Y35" s="6"/>
+      <c r="Z35" s="6"/>
+      <c r="AA35" s="6"/>
+      <c r="AB35" s="6"/>
+      <c r="AC35" s="6"/>
+      <c r="AD35" s="6"/>
+      <c r="AE35" s="6"/>
+      <c r="AF35" s="67"/>
+      <c r="AG35" s="67"/>
+      <c r="AH35" s="67"/>
+      <c r="AI35" s="67"/>
+      <c r="AJ35" s="67"/>
+      <c r="AK35" s="67"/>
+      <c r="AL35" s="31"/>
+    </row>
+    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A36" s="66"/>
+      <c r="B36" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="6"/>
+      <c r="U36" s="6"/>
+      <c r="V36" s="6"/>
+      <c r="W36" s="6"/>
+      <c r="X36" s="6"/>
+      <c r="Y36" s="6"/>
+      <c r="Z36" s="6"/>
+      <c r="AA36" s="6"/>
+      <c r="AB36" s="6"/>
+      <c r="AC36" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD36" s="6"/>
+      <c r="AE36" s="6"/>
+      <c r="AF36" s="67"/>
+      <c r="AG36" s="67"/>
+      <c r="AH36" s="67"/>
+      <c r="AI36" s="67"/>
+      <c r="AJ36" s="67"/>
+      <c r="AK36" s="67"/>
+      <c r="AL36" s="31"/>
+    </row>
+    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A37" s="66"/>
+      <c r="B37" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="6"/>
+      <c r="T37" s="6"/>
+      <c r="U37" s="6"/>
+      <c r="V37" s="6"/>
+      <c r="W37" s="6"/>
+      <c r="X37" s="6"/>
+      <c r="Y37" s="6"/>
+      <c r="Z37" s="6"/>
+      <c r="AA37" s="6"/>
+      <c r="AB37" s="6"/>
+      <c r="AC37" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD37" s="6"/>
+      <c r="AE37" s="6"/>
+      <c r="AF37" s="67"/>
+      <c r="AG37" s="67"/>
+      <c r="AH37" s="67"/>
+      <c r="AI37" s="67"/>
+      <c r="AJ37" s="67"/>
+      <c r="AK37" s="67"/>
+      <c r="AL37" s="31"/>
+    </row>
+    <row r="38" spans="1:38" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="51" t="s">
+      <c r="B38" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="32"/>
-      <c r="N31" s="32"/>
-      <c r="O31" s="32"/>
-      <c r="P31" s="32"/>
-      <c r="Q31" s="32"/>
-      <c r="R31" s="32"/>
-      <c r="S31" s="32"/>
-      <c r="T31" s="32"/>
-      <c r="U31" s="32"/>
-      <c r="V31" s="32"/>
-      <c r="W31" s="32"/>
-      <c r="X31" s="32"/>
-      <c r="Y31" s="32"/>
-      <c r="Z31" s="32"/>
-      <c r="AA31" s="32"/>
-      <c r="AB31" s="32"/>
-      <c r="AC31" s="32"/>
-      <c r="AD31" s="33"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="44"/>
-      <c r="C35" s="45"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="32"/>
+      <c r="L38" s="32"/>
+      <c r="M38" s="32"/>
+      <c r="N38" s="32"/>
+      <c r="O38" s="32"/>
+      <c r="P38" s="32"/>
+      <c r="Q38" s="32"/>
+      <c r="R38" s="32"/>
+      <c r="S38" s="32"/>
+      <c r="T38" s="32"/>
+      <c r="U38" s="32"/>
+      <c r="V38" s="32"/>
+      <c r="W38" s="32"/>
+      <c r="X38" s="32"/>
+      <c r="Y38" s="32"/>
+      <c r="Z38" s="32"/>
+      <c r="AA38" s="32"/>
+      <c r="AB38" s="32"/>
+      <c r="AC38" s="32"/>
+      <c r="AD38" s="32"/>
+      <c r="AE38" s="32"/>
+      <c r="AF38" s="32"/>
+      <c r="AG38" s="32"/>
+      <c r="AH38" s="32"/>
+      <c r="AI38" s="32"/>
+      <c r="AJ38" s="32"/>
+      <c r="AK38" s="32"/>
+      <c r="AL38" s="33"/>
+    </row>
+    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+    </row>
+    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B42" s="44"/>
+      <c r="C42" s="45"/>
+    </row>
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="15">
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="AG1:AL1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A26:A27"/>
     <mergeCell ref="A1:B2"/>
+    <mergeCell ref="K1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:AB1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3179,8 +3817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3528,7 +4166,7 @@
       <c r="H19" s="6"/>
       <c r="I19" s="31"/>
     </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="49" t="s">
         <v>26</v>
       </c>

</xml_diff>